<commit_message>
Working with Multiple Sheets
</commit_message>
<xml_diff>
--- a/Python_for_Spreadsheet_Users/fruit.xlsx
+++ b/Python_for_Spreadsheet_Users/fruit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -411,137 +411,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>0.88</v>
       </c>
       <c r="C2">
-        <v>0.88</v>
-      </c>
-      <c r="D2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3">
+        <v>0.23</v>
       </c>
       <c r="C3">
-        <v>0.23</v>
-      </c>
-      <c r="D3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B4">
+        <v>0.68</v>
       </c>
       <c r="C4">
-        <v>0.68</v>
-      </c>
-      <c r="D4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5">
+        <v>3.98</v>
       </c>
       <c r="C5">
-        <v>3.98</v>
-      </c>
-      <c r="D5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
+      <c r="B6">
+        <v>0.96</v>
       </c>
       <c r="C6">
-        <v>0.96</v>
-      </c>
-      <c r="D6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
+      <c r="B7">
+        <v>5.16</v>
       </c>
       <c r="C7">
-        <v>5.16</v>
-      </c>
-      <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>15</v>
+      <c r="B8">
+        <v>5.27</v>
       </c>
       <c r="C8">
-        <v>5.27</v>
-      </c>
-      <c r="D8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
+      <c r="B9">
+        <v>1.1200000000000001</v>
       </c>
       <c r="C9">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="D9">
         <v>3</v>
       </c>
     </row>
@@ -552,12 +525,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>